<commit_message>
laatste versie van het algorithme
</commit_message>
<xml_diff>
--- a/tijd_gespendeerd.xlsx
+++ b/tijd_gespendeerd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rneyn\Documents\MAI\genetic algorithms\assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2690BD-98C9-4852-85FB-DEE0F599EBD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D02CE31-DC55-4963-AA61-6B7C66D425FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4242" yWindow="1668" windowWidth="17280" windowHeight="9444" xr2:uid="{0DA467F2-FAE9-4887-ABFE-0EDF2B17A4C0}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0DA467F2-FAE9-4887-ABFE-0EDF2B17A4C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">date </t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>schrijven aan het verslag</t>
+  </si>
+  <si>
+    <t>selection operators + writing</t>
+  </si>
+  <si>
+    <t>maken van heuristic crossover + heuristic mutation</t>
   </si>
 </sst>
 </file>
@@ -425,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6661370F-27BC-4764-B1E7-05A2E6FA1C64}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -532,10 +538,32 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2">
+        <v>43815</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2">
+        <v>43819</v>
+      </c>
       <c r="B11">
-        <f>SUM(B2:B9)</f>
-        <v>30</v>
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17">
+        <f>SUM(B2:B16)</f>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>